<commit_message>
This is the correct file
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -1,30 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gordo\Documents\Bellhaven\Spring24\Software Architecture\TrueJimapp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{31D36426-998B-460E-B564-DBDF13896786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE9D8387-DD6B-4A6B-BA7F-A2B9CA50D5C1}"/>
   </bookViews>
   <sheets>
-    <sheet name="ورقة1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -85,7 +102,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -97,7 +114,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -114,7 +131,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -144,12 +161,29 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -179,6 +213,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -330,12 +381,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D65CEEB8-7878-4848-A129-9FF8853DD83C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
The base logic works without interaction with the user
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -1,54 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gordo\Documents\Bellhaven\Spring24\Software Architecture\TrueJimapp\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{31D36426-998B-460E-B564-DBDF13896786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE9D8387-DD6B-4A6B-BA7F-A2B9CA50D5C1}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -66,22 +48,82 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -381,13 +423,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D65CEEB8-7878-4848-A129-9FF8853DD83C}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Phone</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>John Doe</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>123-456-7890</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>john@example.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Jane Smith</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>987-654-3210</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>jane@example.com</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a menu for the user, still working in organization.
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,6 +487,23 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Henry E Jones</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>000-000-0000</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>hjones@belhaven.edu</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new Jim requests and fixed the name separation.
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -1,36 +1,93 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gordo\Documents\Bellhaven\Spring24\Software Architecture\TrueJimapp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FE97F0-72B5-4C6A-965E-854206D7ABAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+  <si>
+    <t>F.Name</t>
+  </si>
+  <si>
+    <t>L.Name</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Birthday</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>123-456-7890</t>
+  </si>
+  <si>
+    <t>March 12 2001</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>987-654-3210</t>
+  </si>
+  <si>
+    <t>February 05 2005</t>
+  </si>
+  <si>
+    <t>Abraham</t>
+  </si>
+  <si>
+    <t>Lopez-Gonzalez</t>
+  </si>
+  <si>
+    <t>443-201-0656</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -49,81 +106,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -423,85 +421,73 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Phone</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>John Doe</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>123-456-7890</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>john@example.com</t>
-        </is>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Jane Smith</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>987-654-3210</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>jane@example.com</t>
-        </is>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Henry E Jones</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>000-000-0000</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>hjones@belhaven.edu</t>
-        </is>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor changes to notes
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -1,93 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gordo\Documents\Bellhaven\Spring24\Software Architecture\TrueJimapp\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FE97F0-72B5-4C6A-965E-854206D7ABAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
-  <si>
-    <t>F.Name</t>
-  </si>
-  <si>
-    <t>L.Name</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Birthday</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Doe</t>
-  </si>
-  <si>
-    <t>123-456-7890</t>
-  </si>
-  <si>
-    <t>March 12 2001</t>
-  </si>
-  <si>
-    <t>Jane</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>987-654-3210</t>
-  </si>
-  <si>
-    <t>February 05 2005</t>
-  </si>
-  <si>
-    <t>Abraham</t>
-  </si>
-  <si>
-    <t>Lopez-Gonzalez</t>
-  </si>
-  <si>
-    <t>443-201-0656</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -106,22 +51,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -421,73 +425,177 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" customWidth="1"/>
+    <col width="10.77734375" customWidth="1" min="1" max="1"/>
+    <col width="17.88671875" customWidth="1" min="2" max="2"/>
+    <col width="15.33203125" customWidth="1" min="3" max="3"/>
+    <col width="18.109375" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>F.Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>L.Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Phone</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Birthday</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Doe</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>123-456-7890</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Mar 12 2001</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Jane</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>987-654-3210</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Feb 05 2005</t>
+        </is>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Abraham</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Lopez-Gonzalez</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>443-201-0656</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Mar 12 2001</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Justin</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Humphrey</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>156-489-1350</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Jun 20 2002</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Bryce</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Ramsure</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>601-486-7595</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Sep 16 2001</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Adams</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>601-153-4598</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Aug 13 2000</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>